<commit_message>
30 de junho 2025
</commit_message>
<xml_diff>
--- a/resultados/suj_1_bloco_1.xlsx
+++ b/resultados/suj_1_bloco_1.xlsx
@@ -423,19 +423,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>21.71994757572047</v>
+        <v>25.98413200434529</v>
       </c>
       <c r="B2">
-        <v>560</v>
+        <v>674</v>
       </c>
       <c r="C2">
-        <v>314</v>
+        <v>568</v>
       </c>
       <c r="D2">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E2">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -443,39 +443,39 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>58.06828902057594</v>
+        <v>19.95105704378432</v>
       </c>
       <c r="B3">
-        <v>878</v>
+        <v>907</v>
       </c>
       <c r="C3">
-        <v>295</v>
+        <v>528</v>
       </c>
       <c r="D3">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E3">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>81.11201359596156</v>
+        <v>122.6395717848804</v>
       </c>
       <c r="B4">
-        <v>979</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>298</v>
+        <v>642</v>
       </c>
       <c r="D4">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E4">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -483,59 +483,59 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>6.124001390613428</v>
+        <v>123.7064184900456</v>
       </c>
       <c r="B5">
-        <v>666</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>359</v>
+        <v>663</v>
       </c>
       <c r="D5">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E5">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>68.52381660377139</v>
+        <v>30.37104468118742</v>
       </c>
       <c r="B6">
-        <v>931</v>
+        <v>1001</v>
       </c>
       <c r="C6">
-        <v>351</v>
+        <v>479</v>
       </c>
       <c r="D6">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E6">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>6.178037744147358</v>
+        <v>26.96379937672894</v>
       </c>
       <c r="B7">
-        <v>620</v>
+        <v>649</v>
       </c>
       <c r="C7">
-        <v>377</v>
+        <v>547</v>
       </c>
       <c r="D7">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E7">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -543,19 +543,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>89.53879079159645</v>
+        <v>70.46607276494409</v>
       </c>
       <c r="B8">
-        <v>1020</v>
+        <v>338</v>
       </c>
       <c r="C8">
-        <v>378</v>
+        <v>544</v>
       </c>
       <c r="D8">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E8">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -563,39 +563,39 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>3.068777540251319</v>
+        <v>51.97877640881225</v>
       </c>
       <c r="B9">
-        <v>647</v>
+        <v>452</v>
       </c>
       <c r="C9">
-        <v>371</v>
+        <v>441</v>
       </c>
       <c r="D9">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E9">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>89.16680617154491</v>
+        <v>119.530350585183</v>
       </c>
       <c r="B10">
-        <v>1008</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>450</v>
+        <v>474</v>
       </c>
       <c r="D10">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E10">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -603,22 +603,22 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>0.5262910062702096</v>
+        <v>128.4761038825038</v>
       </c>
       <c r="B11">
-        <v>638</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>361</v>
+        <v>767</v>
       </c>
       <c r="D11">
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="E11">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4 de julho de 2025
</commit_message>
<xml_diff>
--- a/resultados/suj_1_bloco_1.xlsx
+++ b/resultados/suj_1_bloco_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>erro_radial_cm</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>bucar</t>
-  </si>
-  <si>
-    <t>nao_busque</t>
   </si>
   <si>
     <t>busque</t>
@@ -423,13 +420,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>25.98413200434529</v>
+        <v>37.6529892109601</v>
       </c>
       <c r="B2">
-        <v>674</v>
+        <v>711</v>
       </c>
       <c r="C2">
-        <v>568</v>
+        <v>619</v>
       </c>
       <c r="D2">
         <v>800</v>
@@ -443,13 +440,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>19.95105704378432</v>
+        <v>87.23174527890686</v>
       </c>
       <c r="B3">
-        <v>907</v>
+        <v>424</v>
       </c>
       <c r="C3">
-        <v>528</v>
+        <v>689</v>
       </c>
       <c r="D3">
         <v>800</v>
@@ -463,13 +460,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>122.6395717848804</v>
+        <v>156.2591062507433</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>642</v>
+        <v>444</v>
       </c>
       <c r="D4">
         <v>800</v>
@@ -478,18 +475,18 @@
         <v>448</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>123.7064184900456</v>
+        <v>158.5072909037546</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>663</v>
+        <v>590</v>
       </c>
       <c r="D5">
         <v>800</v>
@@ -498,18 +495,18 @@
         <v>448</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>30.37104468118742</v>
+        <v>155.6952038123114</v>
       </c>
       <c r="B6">
-        <v>1001</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="D6">
         <v>800</v>
@@ -523,13 +520,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>26.96379937672894</v>
+        <v>123.6853652880928</v>
       </c>
       <c r="B7">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="C7">
-        <v>547</v>
+        <v>625</v>
       </c>
       <c r="D7">
         <v>800</v>
@@ -543,13 +540,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>70.46607276494409</v>
+        <v>33.15462804192198</v>
       </c>
       <c r="B8">
-        <v>338</v>
+        <v>707</v>
       </c>
       <c r="C8">
-        <v>544</v>
+        <v>590</v>
       </c>
       <c r="D8">
         <v>800</v>
@@ -558,18 +555,18 @@
         <v>448</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>51.97877640881225</v>
+        <v>163.3186278728956</v>
       </c>
       <c r="B9">
-        <v>452</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>441</v>
+        <v>704</v>
       </c>
       <c r="D9">
         <v>800</v>
@@ -578,18 +575,18 @@
         <v>448</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>119.530350585183</v>
+        <v>56.29359121085295</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>524</v>
       </c>
       <c r="C10">
-        <v>474</v>
+        <v>531</v>
       </c>
       <c r="D10">
         <v>800</v>
@@ -598,18 +595,18 @@
         <v>448</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>128.4761038825038</v>
+        <v>105.0520715571112</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>307</v>
       </c>
       <c r="C11">
-        <v>767</v>
+        <v>663</v>
       </c>
       <c r="D11">
         <v>800</v>
@@ -618,7 +615,7 @@
         <v>448</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>